<commit_message>
En lille opdatering i tidsplan
</commit_message>
<xml_diff>
--- a/Tidsplan.xlsx
+++ b/Tidsplan.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Project Planner</t>
   </si>
@@ -154,42 +154,6 @@
     <t>Samarbejdskontrakt</t>
   </si>
   <si>
-    <t>Kravspecifikation</t>
-  </si>
-  <si>
-    <t>Elaboration 2</t>
-  </si>
-  <si>
-    <t>Grundlæggende design</t>
-  </si>
-  <si>
-    <t>Implementering PoC</t>
-  </si>
-  <si>
-    <t>Foranalyse</t>
-  </si>
-  <si>
-    <t>System arkitektur</t>
-  </si>
-  <si>
-    <t>Design…</t>
-  </si>
-  <si>
-    <t>Implementering</t>
-  </si>
-  <si>
-    <t>Review kravspec mm.</t>
-  </si>
-  <si>
-    <t>Review proces mm.</t>
-  </si>
-  <si>
-    <t>Construction 1</t>
-  </si>
-  <si>
-    <t>Design..</t>
-  </si>
-  <si>
     <t>Projektbeskrivelse</t>
   </si>
   <si>
@@ -203,6 +167,24 @@
   </si>
   <si>
     <t>Projekt opsætning (latex, scrumwise, mm.)</t>
+  </si>
+  <si>
+    <t>Krav til anden sprint</t>
+  </si>
+  <si>
+    <t>Krav til webside</t>
+  </si>
+  <si>
+    <t>Arktiktur til webside</t>
+  </si>
+  <si>
+    <t>Design og implementering af v2.</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Projekt Rapport</t>
   </si>
 </sst>
 </file>
@@ -474,13 +456,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -494,7 +476,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -635,26 +617,6 @@
         <bottom style="thin">
           <color theme="0"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -961,8 +923,8 @@
   </sheetPr>
   <dimension ref="B2:BQ34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -977,22 +939,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="B2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="I3" s="8" t="s">
         <v>14</v>
       </c>
@@ -1030,12 +992,12 @@
       </c>
     </row>
     <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
@@ -1235,11 +1197,9 @@
         <v>16</v>
       </c>
       <c r="C10" s="16">
-        <v>6</v>
-      </c>
-      <c r="D10" s="16">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="17">
@@ -1247,8 +1207,8 @@
       </c>
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="22" t="s">
-        <v>29</v>
+      <c r="B11" s="21" t="s">
+        <v>17</v>
       </c>
       <c r="C11" s="16">
         <v>36</v>
@@ -1265,8 +1225,8 @@
       </c>
     </row>
     <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
-        <v>33</v>
+      <c r="B12" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C12" s="16">
         <v>37</v>
@@ -1282,7 +1242,7 @@
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16">
         <v>37</v>
@@ -1300,7 +1260,7 @@
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C14" s="16">
         <v>37</v>
@@ -1316,7 +1276,7 @@
     </row>
     <row r="15" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C15" s="16">
         <v>37</v>
@@ -1332,13 +1292,13 @@
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="16">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D16" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -1348,13 +1308,13 @@
     </row>
     <row r="17" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C17" s="16">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D17" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
@@ -1364,10 +1324,10 @@
     </row>
     <row r="18" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C18" s="16">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D18" s="16">
         <v>1</v>
@@ -1380,10 +1340,10 @@
     </row>
     <row r="19" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C19" s="18">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="D19" s="16">
         <v>2</v>
@@ -1395,9 +1355,6 @@
       </c>
     </row>
     <row r="20" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C20" s="16">
         <v>10</v>
       </c>
@@ -1411,9 +1368,6 @@
       </c>
     </row>
     <row r="21" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C21" s="16">
         <v>10</v>
       </c>
@@ -1427,9 +1381,6 @@
       </c>
     </row>
     <row r="22" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C22" s="16">
         <v>11</v>
       </c>
@@ -1443,9 +1394,6 @@
       </c>
     </row>
     <row r="23" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C23" s="16">
         <v>11</v>
       </c>
@@ -1459,9 +1407,7 @@
       </c>
     </row>
     <row r="24" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="B24" s="15"/>
       <c r="C24" s="16">
         <v>11</v>
       </c>
@@ -1475,9 +1421,7 @@
       </c>
     </row>
     <row r="25" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
-        <v>27</v>
-      </c>
+      <c r="B25" s="15"/>
       <c r="C25" s="16">
         <v>12</v>
       </c>
@@ -1491,9 +1435,7 @@
       </c>
     </row>
     <row r="26" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
-        <v>22</v>
-      </c>
+      <c r="B26" s="15"/>
       <c r="C26" s="16">
         <v>12</v>
       </c>
@@ -1507,9 +1449,6 @@
       </c>
     </row>
     <row r="27" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
@@ -1524,9 +1463,7 @@
       </c>
     </row>
     <row r="28" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="B28" s="15"/>
       <c r="C28" s="16">
         <v>0</v>
       </c>
@@ -1542,9 +1479,7 @@
       </c>
     </row>
     <row r="29" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15" t="s">
-        <v>26</v>
-      </c>
+      <c r="B29" s="15"/>
       <c r="C29" s="16">
         <v>17</v>
       </c>
@@ -1574,7 +1509,7 @@
       <c r="G30" s="17">
         <v>0</v>
       </c>
-      <c r="AD30" s="21"/>
+      <c r="AD30" s="20"/>
     </row>
     <row r="31" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15"/>
@@ -1591,13 +1526,11 @@
       <c r="G31" s="17">
         <v>0</v>
       </c>
-      <c r="AD31" s="21"/>
+      <c r="AD31" s="20"/>
     </row>
     <row r="32" spans="2:30" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="15"/>
-      <c r="C32" s="16">
-        <v>0</v>
-      </c>
+      <c r="C32" s="16"/>
       <c r="D32" s="16">
         <v>0</v>
       </c>
@@ -1608,36 +1541,44 @@
       <c r="G32" s="17">
         <v>0</v>
       </c>
-      <c r="AD32" s="21"/>
+      <c r="AD32" s="20"/>
     </row>
     <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15"/>
+      <c r="B33" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="C33" s="16">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D33" s="16">
         <v>0</v>
       </c>
       <c r="E33" s="16">
-        <v>0</v>
-      </c>
-      <c r="F33" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="F33" s="16">
+        <v>10</v>
+      </c>
       <c r="G33" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="15"/>
+      <c r="B34" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C34" s="16">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="D34" s="16">
         <v>0</v>
       </c>
       <c r="E34" s="16">
-        <v>0</v>
-      </c>
-      <c r="F34" s="16"/>
+        <v>37</v>
+      </c>
+      <c r="F34" s="16">
+        <v>10</v>
+      </c>
       <c r="G34" s="17">
         <v>0</v>
       </c>

</xml_diff>